<commit_message>
feat: convert id int to str
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -512,11 +512,15 @@
         </is>
       </c>
       <c r="G2" t="inlineStr"/>
-      <c r="H2" t="n">
-        <v>1771107170</v>
-      </c>
-      <c r="I2" t="n">
-        <v>55095</v>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>1771107170</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>55095</t>
+        </is>
       </c>
     </row>
     <row r="3">
@@ -551,11 +555,15 @@
         </is>
       </c>
       <c r="G3" t="inlineStr"/>
-      <c r="H3" t="n">
-        <v>135926598</v>
-      </c>
-      <c r="I3" t="n">
-        <v>55095</v>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>135926598</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>55095</t>
+        </is>
       </c>
     </row>
     <row r="4">
@@ -590,11 +598,15 @@
         </is>
       </c>
       <c r="G4" t="inlineStr"/>
-      <c r="H4" t="n">
-        <v>1036184051</v>
-      </c>
-      <c r="I4" t="n">
-        <v>54984</v>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>1036184051</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>54984</t>
+        </is>
       </c>
     </row>
     <row r="5">
@@ -629,11 +641,15 @@
         </is>
       </c>
       <c r="G5" t="inlineStr"/>
-      <c r="H5" t="n">
-        <v>1598577710</v>
-      </c>
-      <c r="I5" t="n">
-        <v>55049</v>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>1598577710</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>55049</t>
+        </is>
       </c>
     </row>
     <row r="6">
@@ -668,11 +684,15 @@
         </is>
       </c>
       <c r="G6" t="inlineStr"/>
-      <c r="H6" t="n">
-        <v>1861598385</v>
-      </c>
-      <c r="I6" t="n">
-        <v>54833</v>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>1861598385</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>54833</t>
+        </is>
       </c>
     </row>
     <row r="7">
@@ -707,11 +727,15 @@
         </is>
       </c>
       <c r="G7" t="inlineStr"/>
-      <c r="H7" t="n">
-        <v>1475197204</v>
-      </c>
-      <c r="I7" t="n">
-        <v>55178</v>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>1475197204</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>55178</t>
+        </is>
       </c>
     </row>
     <row r="8">
@@ -746,11 +770,15 @@
         </is>
       </c>
       <c r="G8" t="inlineStr"/>
-      <c r="H8" t="n">
-        <v>1218724165</v>
-      </c>
-      <c r="I8" t="n">
-        <v>55095</v>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>1218724165</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>55095</t>
+        </is>
       </c>
     </row>
     <row r="9">
@@ -785,11 +813,15 @@
         </is>
       </c>
       <c r="G9" t="inlineStr"/>
-      <c r="H9" t="n">
-        <v>1335747696</v>
-      </c>
-      <c r="I9" t="n">
-        <v>55219</v>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>1335747696</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>55219</t>
+        </is>
       </c>
     </row>
     <row r="10">
@@ -828,11 +860,15 @@
           <t>문화가있는날</t>
         </is>
       </c>
-      <c r="H10" t="n">
-        <v>710390883</v>
-      </c>
-      <c r="I10" t="n">
-        <v>54984</v>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>710390883</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>54984</t>
+        </is>
       </c>
     </row>
     <row r="11">
@@ -867,11 +903,15 @@
         </is>
       </c>
       <c r="G11" t="inlineStr"/>
-      <c r="H11" t="n">
-        <v>421495536</v>
-      </c>
-      <c r="I11" t="n">
-        <v>55049</v>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>421495536</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>55049</t>
+        </is>
       </c>
     </row>
     <row r="12">
@@ -910,11 +950,15 @@
           <t>문화가 있는 날</t>
         </is>
       </c>
-      <c r="H12" t="n">
-        <v>328352251</v>
-      </c>
-      <c r="I12" t="n">
-        <v>54833</v>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>328352251</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>54833</t>
+        </is>
       </c>
     </row>
     <row r="13">
@@ -949,11 +993,15 @@
         </is>
       </c>
       <c r="G13" t="inlineStr"/>
-      <c r="H13" t="n">
-        <v>661594315</v>
-      </c>
-      <c r="I13" t="n">
-        <v>55178</v>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>661594315</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>55178</t>
+        </is>
       </c>
     </row>
     <row r="14">
@@ -988,11 +1036,15 @@
         </is>
       </c>
       <c r="G14" t="inlineStr"/>
-      <c r="H14" t="n">
-        <v>501053668</v>
-      </c>
-      <c r="I14" t="n">
-        <v>55219</v>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>501053668</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>55219</t>
+        </is>
       </c>
     </row>
     <row r="15">
@@ -1027,11 +1079,15 @@
         </is>
       </c>
       <c r="G15" t="inlineStr"/>
-      <c r="H15" t="n">
-        <v>690847578</v>
-      </c>
-      <c r="I15" t="n">
-        <v>54984</v>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>690847578</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>54984</t>
+        </is>
       </c>
     </row>
     <row r="16">
@@ -1066,11 +1122,15 @@
         </is>
       </c>
       <c r="G16" t="inlineStr"/>
-      <c r="H16" t="n">
-        <v>185395172</v>
-      </c>
-      <c r="I16" t="n">
-        <v>55049</v>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>185395172</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>55049</t>
+        </is>
       </c>
     </row>
     <row r="17">
@@ -1105,11 +1165,15 @@
         </is>
       </c>
       <c r="G17" t="inlineStr"/>
-      <c r="H17" t="n">
-        <v>41766066</v>
-      </c>
-      <c r="I17" t="n">
-        <v>54833</v>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>41766066</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>54833</t>
+        </is>
       </c>
     </row>
     <row r="18">
@@ -1144,11 +1208,15 @@
         </is>
       </c>
       <c r="G18" t="inlineStr"/>
-      <c r="H18" t="n">
-        <v>1864932577</v>
-      </c>
-      <c r="I18" t="n">
-        <v>55178</v>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>1864932577</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>55178</t>
+        </is>
       </c>
     </row>
     <row r="19">
@@ -1183,11 +1251,15 @@
         </is>
       </c>
       <c r="G19" t="inlineStr"/>
-      <c r="H19" t="n">
-        <v>1297184699</v>
-      </c>
-      <c r="I19" t="n">
-        <v>55219</v>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>1297184699</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>55219</t>
+        </is>
       </c>
     </row>
     <row r="20">
@@ -1226,11 +1298,15 @@
           <t>스페셜</t>
         </is>
       </c>
-      <c r="H20" t="n">
-        <v>1761394353</v>
-      </c>
-      <c r="I20" t="n">
-        <v>55319</v>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>1761394353</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>55319</t>
+        </is>
       </c>
     </row>
     <row r="21">
@@ -1269,11 +1345,15 @@
           <t>스페셜</t>
         </is>
       </c>
-      <c r="H21" t="n">
-        <v>115833620</v>
-      </c>
-      <c r="I21" t="n">
-        <v>55321</v>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>115833620</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>55321</t>
+        </is>
       </c>
     </row>
     <row r="22">
@@ -1312,11 +1392,15 @@
           <t>4구간</t>
         </is>
       </c>
-      <c r="H22" t="n">
-        <v>1147473818</v>
-      </c>
-      <c r="I22" t="n">
-        <v>55319</v>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>1147473818</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>55319</t>
+        </is>
       </c>
     </row>
     <row r="23">
@@ -1355,11 +1439,15 @@
           <t>4구간</t>
         </is>
       </c>
-      <c r="H23" t="n">
-        <v>300409083</v>
-      </c>
-      <c r="I23" t="n">
-        <v>55321</v>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>300409083</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>55321</t>
+        </is>
       </c>
     </row>
     <row r="24">
@@ -1398,11 +1486,15 @@
           <t>4구간</t>
         </is>
       </c>
-      <c r="H24" t="n">
-        <v>2091072971</v>
-      </c>
-      <c r="I24" t="n">
-        <v>55319</v>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>2091072971</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>55319</t>
+        </is>
       </c>
     </row>
     <row r="25">
@@ -1441,11 +1533,15 @@
           <t>4구간</t>
         </is>
       </c>
-      <c r="H25" t="n">
-        <v>1532447433</v>
-      </c>
-      <c r="I25" t="n">
-        <v>55321</v>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>1532447433</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>55321</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>